<commit_message>
Hinzufügen der Team index Dateien und update Test
</commit_message>
<xml_diff>
--- a/documents/project management/Test/Abnahmetest_Go Happy_gesamt.xlsx
+++ b/documents/project management/Test/Abnahmetest_Go Happy_gesamt.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -290,6 +290,36 @@
   </si>
   <si>
     <t>Was passiert hier?</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Ort an und klickt auf den "Zurück-Pfeil". Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Wochentag an und klickt auf den "Zurück-Pfeil". Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Radius an und klickt auf den "Zurück-Pfeil". Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Uhrzeit an und klickt auf den "Zurück-Pfeil". Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Verweilszeit an und klickt auf den "Zurück-Pfeil". Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen</t>
+  </si>
+  <si>
+    <t>Der Anwender öffnet die Web-Anwendung und betätigt den "Go Happy"-Button und es werden keine Bars, auf den die Parameter zutreffen, gefunden.</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Ort an und klickt auf den "Zurück-Pfeil".  Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen und eine oder mehrer Bars passen nicht mehr zu den eingestellten Parametern.</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Radius an und klickt auf den "Zurück-Pfeil".  Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen und eine oder mehrere Bars passen nicht mehr zu den eingestellten Parametern.</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Uhrzeit an und klickt auf den "Zurück-Pfeil".  Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen und eine oder mehrere Bars passennicht mehr zu den eingestellten Parametern.</t>
+  </si>
+  <si>
+    <t>Der Anwender hat sich eine Route erstellen lassen, klickt auf das "Options-Icon" und passt die Einstellung Verweilzeit an und klickt auf den "Zurück-Pfeil".  Daraufhin wird der "Aktualisierungs-Button" betätigt, um die Einstellungen zu übernehmen und eine oder mehrere Bars passen nicht mehr zu den eingestellten Parametern.</t>
   </si>
 </sst>
 </file>
@@ -767,10 +797,126 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
-      <border outline="0">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -781,6 +927,13 @@
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -934,6 +1087,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -941,12 +1100,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
@@ -1099,6 +1252,26 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1120,149 +1293,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
@@ -1309,8 +1339,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:K40" totalsRowShown="0">
-  <autoFilter ref="A2:K40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle4" displayName="Tabelle4" ref="A2:K39" totalsRowShown="0">
+  <autoFilter ref="A2:K39"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID" dataDxfId="31"/>
     <tableColumn id="2" name="Testszenario" dataDxfId="30"/>
@@ -1341,42 +1371,42 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E40" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="19" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A2:E40" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A2:E40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="18"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="17"/>
+    <tableColumn id="1" name="ID" dataDxfId="17"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="16"/>
     <tableColumn id="3" name="Erwartungen"/>
-    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="16"/>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="15"/>
+    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="15"/>
+    <tableColumn id="5" name="Kommentar Backend" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle14" displayName="Tabelle14" ref="A2:E40" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle14" displayName="Tabelle14" ref="A2:E40" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A2:E40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="13"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="12"/>
+    <tableColumn id="1" name="ID" dataDxfId="10"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="9"/>
     <tableColumn id="3" name="Erwartungen"/>
-    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="11"/>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="10"/>
+    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="8"/>
+    <tableColumn id="5" name="Kommentar Backend" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle146" displayName="Tabelle146" ref="A2:E40" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle146" displayName="Tabelle146" ref="A2:E40" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A2:E40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="6"/>
-    <tableColumn id="2" name="Testszenario" dataDxfId="5"/>
+    <tableColumn id="1" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" name="Testszenario" dataDxfId="2"/>
     <tableColumn id="3" name="Erwartungen"/>
-    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="4"/>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="3"/>
+    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="1"/>
+    <tableColumn id="5" name="Kommentar Backend" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1704,10 +1734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1807,7 +1837,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>9</v>
@@ -1839,12 +1869,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="30">
+    <row r="5" spans="1:11" ht="45">
       <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -1876,12 +1906,12 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="30">
+    <row r="6" spans="1:11" ht="60">
       <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
@@ -1913,12 +1943,12 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="30">
+    <row r="7" spans="1:11" ht="45">
       <c r="A7" s="16">
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
@@ -1950,12 +1980,12 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="30">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="16">
         <v>6</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -1987,12 +2017,12 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="30">
+    <row r="9" spans="1:11" ht="60">
       <c r="A9" s="16">
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -2029,7 +2059,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>61</v>
@@ -2066,7 +2096,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>61</v>
@@ -2103,7 +2133,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>61</v>
@@ -2140,7 +2170,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>61</v>
@@ -2392,15 +2422,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" ht="30">
+    <row r="20" spans="1:11" ht="30">
       <c r="A20" s="16">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>66</v>
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D20" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2411,31 +2441,33 @@
         <v>0</v>
       </c>
       <c r="F20" s="11">
-        <f>Frontend!D21</f>
+        <f>Frontend!D20</f>
         <v>0</v>
       </c>
       <c r="G20" s="11">
-        <f>Frontend!E21</f>
+        <f>Frontend!E20</f>
         <v>0</v>
       </c>
       <c r="H20" s="11">
-        <f>Design!D21</f>
+        <f>Design!D20</f>
         <v>0</v>
       </c>
       <c r="I20" s="11">
-        <f>Design!E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30">
+        <f>Design!E20</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="45">
       <c r="A21" s="16">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2445,20 +2477,20 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F21" s="11">
-        <f>Frontend!D20</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <f>Frontend!E20</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="11">
-        <f>Design!D20</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="11">
-        <f>Design!E20</f>
+      <c r="F21" s="1">
+        <f>Frontend!D17</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f>Frontend!E17</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <f>Design!D17</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <f>Design!E17</f>
         <v>0</v>
       </c>
       <c r="J21" s="1"/>
@@ -2466,13 +2498,13 @@
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" s="16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2483,19 +2515,19 @@
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <f>Frontend!D17</f>
+        <f>Frontend!D18</f>
         <v>0</v>
       </c>
       <c r="G22" s="1">
-        <f>Frontend!E17</f>
+        <f>Frontend!E18</f>
         <v>0</v>
       </c>
       <c r="H22" s="1">
-        <f>Design!D17</f>
+        <f>Design!D18</f>
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <f>Design!E17</f>
+        <f>Design!E18</f>
         <v>0</v>
       </c>
       <c r="J22" s="1"/>
@@ -2503,13 +2535,13 @@
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="16">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2520,19 +2552,19 @@
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <f>Frontend!D18</f>
+        <f>Frontend!D19</f>
         <v>0</v>
       </c>
       <c r="G23" s="1">
-        <f>Frontend!E18</f>
+        <f>Frontend!E19</f>
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <f>Design!D18</f>
+        <f>Design!D19</f>
         <v>0</v>
       </c>
       <c r="I23" s="1">
-        <f>Design!E18</f>
+        <f>Design!E19</f>
         <v>0</v>
       </c>
       <c r="J23" s="1"/>
@@ -2540,13 +2572,13 @@
     </row>
     <row r="24" spans="1:11" ht="45">
       <c r="A24" s="16">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2556,34 +2588,34 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F24" s="1">
-        <f>Frontend!D19</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <f>Frontend!E19</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <f>Design!D19</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <f>Design!E19</f>
+      <c r="F24" s="11">
+        <f>Frontend!D26</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <f>Frontend!E26</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <f>Design!D26</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="11">
+        <f>Design!E26</f>
         <v>0</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="45">
+    <row r="25" spans="1:11" ht="30">
       <c r="A25" s="16">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2593,34 +2625,34 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F25" s="11">
-        <f>Frontend!D26</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="11">
-        <f>Frontend!E26</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="11">
-        <f>Design!D26</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
-        <f>Design!E26</f>
+      <c r="F25" s="1">
+        <f>Frontend!D20</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <f>Frontend!E20</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f>Design!D20</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <f>Design!E20</f>
         <v>0</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="30">
+    <row r="26" spans="1:11" ht="45">
       <c r="A26" s="16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2631,33 +2663,33 @@
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <f>Frontend!D20</f>
+        <f>Frontend!D21</f>
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <f>Frontend!E20</f>
+        <f>Frontend!E21</f>
         <v>0</v>
       </c>
       <c r="H26" s="1">
-        <f>Design!D20</f>
+        <f>Design!D21</f>
         <v>0</v>
       </c>
       <c r="I26" s="1">
-        <f>Design!E20</f>
+        <f>Design!E21</f>
         <v>0</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="45">
+    <row r="27" spans="1:11" ht="60">
       <c r="A27" s="16">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2667,34 +2699,34 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F27" s="1">
-        <f>Frontend!D21</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <f>Frontend!E21</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <f>Design!D21</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <f>Design!E21</f>
+      <c r="F27" s="11">
+        <f>Frontend!D29</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <f>Frontend!E29</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <f>Design!D29</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="11">
+        <f>Design!E29</f>
         <v>0</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="60">
+    <row r="28" spans="1:11" ht="45">
       <c r="A28" s="16">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2704,20 +2736,20 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F28" s="11">
-        <f>Frontend!D29</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <f>Frontend!E29</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <f>Design!D29</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
-        <f>Design!E29</f>
+      <c r="F28" s="1">
+        <f>Frontend!D22</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <f>Frontend!E22</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <f>Design!D22</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <f>Design!E22</f>
         <v>0</v>
       </c>
       <c r="J28" s="1"/>
@@ -2725,13 +2757,13 @@
     </row>
     <row r="29" spans="1:11" ht="45">
       <c r="A29" s="16">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2742,19 +2774,19 @@
         <v>0</v>
       </c>
       <c r="F29" s="1">
-        <f>Frontend!D22</f>
+        <f>Frontend!D23</f>
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <f>Frontend!E22</f>
+        <f>Frontend!E23</f>
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <f>Design!D22</f>
+        <f>Design!D23</f>
         <v>0</v>
       </c>
       <c r="I29" s="1">
-        <f>Design!E22</f>
+        <f>Design!E23</f>
         <v>0</v>
       </c>
       <c r="J29" s="1"/>
@@ -2762,13 +2794,13 @@
     </row>
     <row r="30" spans="1:11" ht="45">
       <c r="A30" s="16">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2779,33 +2811,33 @@
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <f>Frontend!D23</f>
+        <f>Frontend!D24</f>
         <v>0</v>
       </c>
       <c r="G30" s="1">
-        <f>Frontend!E23</f>
+        <f>Frontend!E24</f>
         <v>0</v>
       </c>
       <c r="H30" s="1">
-        <f>Design!D23</f>
+        <f>Design!D24</f>
         <v>0</v>
       </c>
       <c r="I30" s="1">
-        <f>Design!E23</f>
+        <f>Design!E24</f>
         <v>0</v>
       </c>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="45">
+    <row r="31" spans="1:11" ht="30">
       <c r="A31" s="16">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D31" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2816,19 +2848,19 @@
         <v>0</v>
       </c>
       <c r="F31" s="1">
-        <f>Frontend!D24</f>
+        <f>Frontend!D25</f>
         <v>0</v>
       </c>
       <c r="G31" s="1">
-        <f>Frontend!E24</f>
+        <f>Frontend!E25</f>
         <v>0</v>
       </c>
       <c r="H31" s="1">
-        <f>Design!D24</f>
+        <f>Design!D25</f>
         <v>0</v>
       </c>
       <c r="I31" s="1">
-        <f>Design!E24</f>
+        <f>Design!E25</f>
         <v>0</v>
       </c>
       <c r="J31" s="1"/>
@@ -2836,13 +2868,13 @@
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="16">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>74</v>
+        <v>55</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D32" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2852,34 +2884,34 @@
         <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
         <v>0</v>
       </c>
-      <c r="F32" s="1">
-        <f>Frontend!D25</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <f>Frontend!E25</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
-        <f>Design!D25</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <f>Design!E25</f>
+      <c r="F32" s="11">
+        <f>Frontend!D26</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="11">
+        <f>Frontend!E26</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="11">
+        <f>Design!D26</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="11">
+        <f>Design!E26</f>
         <v>0</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="30">
+    <row r="33" spans="1:11" ht="45">
       <c r="A33" s="16">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2890,33 +2922,33 @@
         <v>0</v>
       </c>
       <c r="F33" s="11">
-        <f>Frontend!D26</f>
+        <f>Frontend!D27</f>
         <v>0</v>
       </c>
       <c r="G33" s="11">
-        <f>Frontend!E26</f>
+        <f>Frontend!E27</f>
         <v>0</v>
       </c>
       <c r="H33" s="11">
-        <f>Design!D26</f>
+        <f>Design!D27</f>
         <v>0</v>
       </c>
       <c r="I33" s="11">
-        <f>Design!E26</f>
+        <f>Design!E27</f>
         <v>0</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="45">
+    <row r="34" spans="1:11" ht="30">
       <c r="A34" s="16">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2927,19 +2959,19 @@
         <v>0</v>
       </c>
       <c r="F34" s="11">
-        <f>Frontend!D27</f>
+        <f>Frontend!D28</f>
         <v>0</v>
       </c>
       <c r="G34" s="11">
-        <f>Frontend!E27</f>
+        <f>Frontend!E28</f>
         <v>0</v>
       </c>
       <c r="H34" s="11">
-        <f>Design!D27</f>
+        <f>Design!D28</f>
         <v>0</v>
       </c>
       <c r="I34" s="11">
-        <f>Design!E27</f>
+        <f>Design!E28</f>
         <v>0</v>
       </c>
       <c r="J34" s="1"/>
@@ -2947,13 +2979,13 @@
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="16">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -2964,33 +2996,33 @@
         <v>0</v>
       </c>
       <c r="F35" s="11">
-        <f>Frontend!D28</f>
+        <f>Frontend!D29</f>
         <v>0</v>
       </c>
       <c r="G35" s="11">
-        <f>Frontend!E28</f>
+        <f>Frontend!E29</f>
         <v>0</v>
       </c>
       <c r="H35" s="11">
-        <f>Design!D28</f>
+        <f>Design!D29</f>
         <v>0</v>
       </c>
       <c r="I35" s="11">
-        <f>Design!E28</f>
+        <f>Design!E29</f>
         <v>0</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="30">
+    <row r="36" spans="1:11" ht="45">
       <c r="A36" s="16">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -3001,33 +3033,33 @@
         <v>0</v>
       </c>
       <c r="F36" s="11">
-        <f>Frontend!D29</f>
+        <f>Frontend!D30</f>
         <v>0</v>
       </c>
       <c r="G36" s="11">
-        <f>Frontend!E29</f>
+        <f>Frontend!E30</f>
         <v>0</v>
       </c>
       <c r="H36" s="11">
-        <f>Design!D29</f>
+        <f>Design!D30</f>
         <v>0</v>
       </c>
       <c r="I36" s="11">
-        <f>Design!E29</f>
+        <f>Design!E30</f>
         <v>0</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="45">
+    <row r="37" spans="1:11" ht="30">
       <c r="A37" s="16">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="D37" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -3038,33 +3070,33 @@
         <v>0</v>
       </c>
       <c r="F37" s="11">
-        <f>Frontend!D30</f>
+        <f>Frontend!D31</f>
         <v>0</v>
       </c>
       <c r="G37" s="11">
-        <f>Frontend!E30</f>
+        <f>Frontend!E31</f>
         <v>0</v>
       </c>
       <c r="H37" s="11">
-        <f>Design!D30</f>
+        <f>Design!D31</f>
         <v>0</v>
       </c>
       <c r="I37" s="11">
-        <f>Design!E30</f>
+        <f>Design!E31</f>
         <v>0</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="30">
+    <row r="38" spans="1:11">
       <c r="A38" s="16">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="D38" s="1">
         <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
@@ -3075,19 +3107,19 @@
         <v>0</v>
       </c>
       <c r="F38" s="11">
-        <f>Frontend!D31</f>
+        <f>Frontend!D32</f>
         <v>0</v>
       </c>
       <c r="G38" s="11">
-        <f>Frontend!E31</f>
+        <f>Frontend!E32</f>
         <v>0</v>
       </c>
       <c r="H38" s="11">
-        <f>Design!D31</f>
+        <f>Design!D32</f>
         <v>0</v>
       </c>
       <c r="I38" s="11">
-        <f>Design!E31</f>
+        <f>Design!E32</f>
         <v>0</v>
       </c>
       <c r="J38" s="1"/>
@@ -3095,10 +3127,10 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="16">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>81</v>
@@ -3112,63 +3144,26 @@
         <v>0</v>
       </c>
       <c r="F39" s="11">
-        <f>Frontend!D32</f>
+        <f>Frontend!D33</f>
         <v>0</v>
       </c>
       <c r="G39" s="11">
-        <f>Frontend!E32</f>
+        <f>Frontend!E33</f>
         <v>0</v>
       </c>
       <c r="H39" s="11">
-        <f>Design!D32</f>
+        <f>Design!D33</f>
         <v>0</v>
       </c>
       <c r="I39" s="11">
-        <f>Design!E32</f>
+        <f>Design!E33</f>
         <v>0</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="16">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="1">
-        <f>Tabelle1[[#This Row],[Ergebnis Backend]]</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <f>Tabelle1[[#This Row],[Kommentar Backend]]</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="11">
-        <f>Frontend!D33</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="11">
-        <f>Frontend!E33</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="11">
-        <f>Design!D33</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="11">
-        <f>Design!E33</f>
-        <v>0</v>
-      </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="F3:F40 H3:H40 J3:J40 D3:D40">
+  <conditionalFormatting sqref="F3:F39 H3:H39 J3:J39 D3:D39">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>